<commit_message>
Added requirements for virtual machine
</commit_message>
<xml_diff>
--- a/samplesheet_to_zlims_wgs_task/results/E250077027_zlims_wgs_samplesheet.xlsx
+++ b/samplesheet_to_zlims_wgs_task/results/E250077027_zlims_wgs_samplesheet.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -53,18 +53,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -557,12 +557,12 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>/mnt/z/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR66_1.fq.gz</t>
+          <t>/storeData/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR66_1.fq.gz</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>/mnt/z/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR66_2.fq.gz</t>
+          <t>/storeData/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR66_2.fq.gz</t>
         </is>
       </c>
       <c r="H3" t="inlineStr"/>
@@ -595,12 +595,12 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>/mnt/z/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR67_1.fq.gz</t>
+          <t>/storeData/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR67_1.fq.gz</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>/mnt/z/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR67_2.fq.gz</t>
+          <t>/storeData/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR67_2.fq.gz</t>
         </is>
       </c>
       <c r="H4" t="inlineStr"/>
@@ -633,12 +633,12 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>/mnt/z/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR70_1.fq.gz</t>
+          <t>/storeData/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR70_1.fq.gz</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>/mnt/z/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR70_2.fq.gz</t>
+          <t>/storeData/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR70_2.fq.gz</t>
         </is>
       </c>
       <c r="H5" t="inlineStr"/>
@@ -671,12 +671,12 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>/mnt/z/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR71_1.fq.gz</t>
+          <t>/storeData/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR71_1.fq.gz</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>/mnt/z/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR71_2.fq.gz</t>
+          <t>/storeData/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR71_2.fq.gz</t>
         </is>
       </c>
       <c r="H6" t="inlineStr"/>
@@ -709,12 +709,12 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>/mnt/z/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR97_1.fq.gz</t>
+          <t>/storeData/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR97_1.fq.gz</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>/mnt/z/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR97_2.fq.gz</t>
+          <t>/storeData/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR97_2.fq.gz</t>
         </is>
       </c>
       <c r="H7" t="inlineStr"/>
@@ -747,12 +747,12 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>/mnt/z/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR104_1.fq.gz</t>
+          <t>/storeData/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR104_1.fq.gz</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>/mnt/z/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR104_2.fq.gz</t>
+          <t>/storeData/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR104_2.fq.gz</t>
         </is>
       </c>
       <c r="H8" t="inlineStr"/>
@@ -785,12 +785,12 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>/mnt/z/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR105_1.fq.gz</t>
+          <t>/storeData/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR105_1.fq.gz</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>/mnt/z/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR105_2.fq.gz</t>
+          <t>/storeData/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR105_2.fq.gz</t>
         </is>
       </c>
       <c r="H9" t="inlineStr"/>
@@ -823,12 +823,12 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>/mnt/z/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR106_1.fq.gz</t>
+          <t>/storeData/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR106_1.fq.gz</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>/mnt/z/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR106_2.fq.gz</t>
+          <t>/storeData/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR106_2.fq.gz</t>
         </is>
       </c>
       <c r="H10" t="inlineStr"/>
@@ -861,12 +861,12 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>/mnt/z/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR107_1.fq.gz</t>
+          <t>/storeData/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR107_1.fq.gz</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>/mnt/z/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR107_2.fq.gz</t>
+          <t>/storeData/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR107_2.fq.gz</t>
         </is>
       </c>
       <c r="H11" t="inlineStr"/>
@@ -899,12 +899,12 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>/mnt/z/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR115_1.fq.gz</t>
+          <t>/storeData/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR115_1.fq.gz</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>/mnt/z/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR115_2.fq.gz</t>
+          <t>/storeData/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR115_2.fq.gz</t>
         </is>
       </c>
       <c r="H12" t="inlineStr"/>
@@ -937,12 +937,12 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>/mnt/z/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR116_1.fq.gz</t>
+          <t>/storeData/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR116_1.fq.gz</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>/mnt/z/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR116_2.fq.gz</t>
+          <t>/storeData/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR116_2.fq.gz</t>
         </is>
       </c>
       <c r="H13" t="inlineStr"/>
@@ -975,17 +975,17 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>/mnt/z/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR117_1.fq.gz</t>
+          <t>/storeData/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR117_1.fq.gz</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>/mnt/z/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR117_2.fq.gz</t>
+          <t>/storeData/ztron/autorunDW/DNBSEQ-T7/R2100610220009/write_fastq_config_1_5/ztron/E250077027_L01_14525/E250077027_L01/E250077027_L01_CIR117_2.fq.gz</t>
         </is>
       </c>
       <c r="H14" t="inlineStr"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>